<commit_message>
Adding manual edits to generator id updates.
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_edits.xlsx
+++ b/data/static_tables/manual_edits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abtassoc-my.sharepoint.com/personal/teagan_goforth_abtassoc_com/Documents/Documents/eGRID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F155C48-3B7E-4B56-A58D-A5D686E642DB}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{548FE47B-F7CC-4BFA-90AA-6EF8BFD94FFE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
   <si>
     <t>plant_id</t>
   </si>
@@ -139,19 +139,13 @@
     <t>8.2</t>
   </si>
   <si>
-    <t>update_numeric</t>
-  </si>
-  <si>
-    <t>update_character</t>
+    <t>8.1999999999999993</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -195,12 +189,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,21 +528,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B152A-9A17-4C98-BF21-937C78FED9AB}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,13 +552,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>7512</v>
       </c>
@@ -580,7 +569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>7512</v>
       </c>
@@ -594,7 +583,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>7512</v>
       </c>
@@ -608,21 +597,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>664</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" s="4">
-        <v>8.1999999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>